<commit_message>
N5 N4 N3 options
</commit_message>
<xml_diff>
--- a/Vocabulary.xlsx
+++ b/Vocabulary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leechehsi/Library/Mobile Documents/com~apple~CloudDocs/Officially_Get_Married/N3_voc_grammar_test_code/dist/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\李哲熙\03_求學\04日文相關\N3_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0824152E-5A36-3A47-8EBB-4080BA9B8760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE3A0A5-5692-4C64-8D8F-D3FC22827A0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="29400" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="341">
   <si>
     <t>單字</t>
   </si>
@@ -816,6 +816,454 @@
   </si>
   <si>
     <t>轉角</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>かばん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>花瓶</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>かびん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>紙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>かみ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>体</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>からだ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>川</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>かわ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>漢字</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>かんじ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>木</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>き</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>北</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>きた</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>喫茶店</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>きっさてん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>切手</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>きって</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>切符</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>きっぷ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>昨日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>きのう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛肉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ぎゅうにく</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛乳</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ぎゅうにゆう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>今日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>きょう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>教室</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>きょうしつ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>兄弟</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>きょうだい</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>去年</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>きょねん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>銀行</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ぎんこう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>薬</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>くすり</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>果物</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>くだもの</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>口</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>くち</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 皮包</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>身體</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>河川</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>樹</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>北方北邊</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>咖啡廳</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>郵票</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>車票</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>昨天</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛奶</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>今天</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>藥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘴巴</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>靴</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>くつ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>靴下</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>くつした</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>国</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>くに</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>車</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>くるま</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>警官</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>けいかん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>今朝</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>けさ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>結婚</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>けっこん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>公園</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>こうえん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>紅茶</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>こうちゃ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>交番</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>こうばん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>声</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>こえ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>午後</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ごご</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>午前</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ごぜん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>こちら</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>今年</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ことし</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>子ども</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>こども</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ご飯</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ごはん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>今月</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>こんげつ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>今週</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>こんしゅう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>今晩</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>こんばん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>鞋子</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>襪子</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>國家</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>車子</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>警察</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>今天早上</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>警察局</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>聲音</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下午</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上午</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(尊敬)這邊</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>小孩子</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>吃飯，飯</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>這星期</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>這個月</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>今晚</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -823,7 +1271,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -844,6 +1292,13 @@
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -881,11 +1336,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1188,22 +1644,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="188" zoomScaleNormal="188" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="188" zoomScaleNormal="188" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1249,7 +1705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1272,7 +1728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1295,7 +1751,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -1315,7 +1771,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1338,7 +1794,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1361,7 +1817,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1381,7 +1837,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1404,7 +1860,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -1424,7 +1880,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1447,7 +1903,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>33</v>
       </c>
@@ -1467,7 +1923,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1490,7 +1946,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1513,7 +1969,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1536,7 +1992,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1559,7 +2015,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>46</v>
       </c>
@@ -1579,7 +2035,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>48</v>
       </c>
@@ -1599,7 +2055,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1622,7 +2078,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1645,7 +2101,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>56</v>
       </c>
@@ -1665,7 +2121,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1688,7 +2144,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>61</v>
       </c>
@@ -1708,7 +2164,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -1731,7 +2187,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -1754,7 +2210,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -1777,7 +2233,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -1800,7 +2256,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -1823,7 +2279,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -1846,7 +2302,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -1869,7 +2325,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -1892,7 +2348,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>87</v>
       </c>
@@ -1915,7 +2371,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -1938,7 +2394,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -1961,7 +2417,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -1984,7 +2440,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -2007,7 +2463,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>100</v>
       </c>
@@ -2030,7 +2486,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>103</v>
       </c>
@@ -2053,7 +2509,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>105</v>
       </c>
@@ -2076,7 +2532,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>108</v>
       </c>
@@ -2099,7 +2555,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>111</v>
       </c>
@@ -2122,7 +2578,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>113</v>
       </c>
@@ -2145,7 +2601,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -2168,7 +2624,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>119</v>
       </c>
@@ -2179,7 +2635,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>120</v>
       </c>
@@ -2190,7 +2646,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>121</v>
       </c>
@@ -2201,7 +2657,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>122</v>
       </c>
@@ -2212,7 +2668,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>123</v>
       </c>
@@ -2223,7 +2679,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>124</v>
       </c>
@@ -2231,7 +2687,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>125</v>
       </c>
@@ -2239,7 +2695,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>131</v>
       </c>
@@ -2250,7 +2706,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>133</v>
       </c>
@@ -2261,7 +2717,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>135</v>
       </c>
@@ -2272,7 +2728,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>137</v>
       </c>
@@ -2283,7 +2739,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>139</v>
       </c>
@@ -2294,7 +2750,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>141</v>
       </c>
@@ -2302,7 +2758,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>142</v>
       </c>
@@ -2310,7 +2766,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>143</v>
       </c>
@@ -2321,7 +2777,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>145</v>
       </c>
@@ -2332,7 +2788,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>147</v>
       </c>
@@ -2343,7 +2799,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>149</v>
       </c>
@@ -2354,7 +2810,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>151</v>
       </c>
@@ -2362,7 +2818,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>152</v>
       </c>
@@ -2370,7 +2826,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>153</v>
       </c>
@@ -2381,7 +2837,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>175</v>
       </c>
@@ -2392,7 +2848,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>177</v>
       </c>
@@ -2400,7 +2856,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>178</v>
       </c>
@@ -2411,7 +2867,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>180</v>
       </c>
@@ -2422,7 +2878,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>182</v>
       </c>
@@ -2433,7 +2889,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>184</v>
       </c>
@@ -2444,7 +2900,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>186</v>
       </c>
@@ -2455,7 +2911,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>188</v>
       </c>
@@ -2466,7 +2922,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>190</v>
       </c>
@@ -2477,7 +2933,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>192</v>
       </c>
@@ -2488,7 +2944,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>194</v>
       </c>
@@ -2499,7 +2955,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>196</v>
       </c>
@@ -2510,7 +2966,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>198</v>
       </c>
@@ -2518,7 +2974,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>199</v>
       </c>
@@ -2529,7 +2985,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>201</v>
       </c>
@@ -2537,7 +2993,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>202</v>
       </c>
@@ -2548,7 +3004,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>203</v>
       </c>
@@ -2559,7 +3015,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>205</v>
       </c>
@@ -2570,7 +3026,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -2581,7 +3037,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>209</v>
       </c>
@@ -2590,10 +3046,467 @@
       </c>
       <c r="C84" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="B85" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C85" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>230</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C86" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C87" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A88" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C88" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C89" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C90" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C91" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A92" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C92" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A93" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C93" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C94" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C95" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A96" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C96" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A97" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C97" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C98" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A99" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C99" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A100" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C100" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A101" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C101" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C102" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C103" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A104" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C104" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A105" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C105" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A106" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C106" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A107" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C107" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A108" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C108" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A109" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C109" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A110" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C110" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A111" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C111" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A112" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C112" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A113" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C113" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A114" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C114" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A115" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C115" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A116" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C116" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A117" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C117" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A118" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C118" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A119" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C119" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="B120" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C120" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A121" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C121" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A122" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C122" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A123" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C123" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A124" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C124" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A125" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C125" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A126" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C126" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>